<commit_message>
AD scripts to generate barcodes; oligoanalyzer output analysis script added
</commit_message>
<xml_diff>
--- a/source_data/Supplementary_Table_1.xlsx
+++ b/source_data/Supplementary_Table_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="580" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="price_details" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="99">
   <si>
     <t>Nextera Flex</t>
   </si>
@@ -325,6 +325,21 @@
   <si>
     <t>SF_vs_Hfv1</t>
   </si>
+  <si>
+    <t>per sample cost SF</t>
+  </si>
+  <si>
+    <t>per sample cost HF v0</t>
+  </si>
+  <si>
+    <t>per sample cost HF v1</t>
+  </si>
+  <si>
+    <t>HF v0 vs SF (fold diff)</t>
+  </si>
+  <si>
+    <t>HF v1 vs SF (fold diff)</t>
+  </si>
 </sst>
 </file>
 
@@ -338,7 +353,7 @@
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -400,8 +415,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,6 +454,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -442,7 +470,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="165">
+  <cellStyleXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -608,8 +636,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -689,12 +739,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -704,8 +753,20 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="165">
+  <cellStyles count="187">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -788,6 +849,17 @@
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -870,6 +942,17 @@
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1207,10 +1290,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I38" sqref="A1:I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1224,6 +1307,7 @@
     <col min="7" max="7" width="11.83203125" customWidth="1"/>
     <col min="8" max="8" width="14.1640625" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1238,7 +1322,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="20"/>
     </row>
-    <row r="2" spans="1:10" ht="60">
+    <row r="2" spans="1:10" ht="45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1642,7 +1726,7 @@
       </c>
       <c r="J16" s="20"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:12">
       <c r="A17" s="28"/>
       <c r="B17" s="29" t="s">
         <v>41</v>
@@ -1674,7 +1758,7 @@
       </c>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:12">
       <c r="A18" s="28"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
@@ -1686,11 +1770,11 @@
       <c r="I18" s="31"/>
       <c r="J18" s="20"/>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1">
-      <c r="A19" s="48" t="s">
+    <row r="19" spans="1:12" ht="15" customHeight="1">
+      <c r="A19" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="46" t="s">
         <v>46</v>
       </c>
       <c r="C19" s="37" t="s">
@@ -1706,23 +1790,23 @@
         <f>(1582/730)*4800</f>
         <v>10402.191780821917</v>
       </c>
-      <c r="G19" s="43">
+      <c r="G19" s="49">
         <f>F19/4800*96</f>
         <v>208.04383561643834</v>
       </c>
-      <c r="H19" s="44">
+      <c r="H19" s="50">
         <f>F19*0.7753</f>
         <v>8064.8192876712319</v>
       </c>
-      <c r="I19" s="44">
+      <c r="I19" s="50">
         <f>G19*0.7753</f>
         <v>161.29638575342466</v>
       </c>
       <c r="J19" s="20"/>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="48"/>
-      <c r="B20" s="47"/>
+    <row r="20" spans="1:12">
+      <c r="A20" s="47"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="26" t="s">
         <v>74</v>
       </c>
@@ -1736,21 +1820,21 @@
         <f>(1582/730)*9600</f>
         <v>20804.383561643834</v>
       </c>
-      <c r="G20" s="41">
+      <c r="G20" s="51">
         <f>F20/4800*96</f>
         <v>416.08767123287669</v>
       </c>
-      <c r="H20" s="42">
+      <c r="H20" s="52">
         <f>F20*0.7753</f>
         <v>16129.638575342464</v>
       </c>
-      <c r="I20" s="42">
+      <c r="I20" s="52">
         <f>G20*0.7753</f>
         <v>322.59277150684932</v>
       </c>
       <c r="J20" s="20"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:12">
       <c r="A21" s="18"/>
       <c r="B21" s="3" t="s">
         <v>48</v>
@@ -1778,7 +1862,7 @@
       </c>
       <c r="J21" s="20"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:12">
       <c r="A22" s="18"/>
       <c r="B22" s="3" t="s">
         <v>51</v>
@@ -1806,7 +1890,7 @@
       </c>
       <c r="J22" s="20"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:12">
       <c r="A23" s="18"/>
       <c r="B23" s="3" t="s">
         <v>53</v>
@@ -1834,7 +1918,7 @@
       </c>
       <c r="J23" s="20"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:12">
       <c r="A24" s="18"/>
       <c r="B24" s="3" t="s">
         <v>55</v>
@@ -1862,7 +1946,7 @@
       </c>
       <c r="J24" s="20"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:12">
       <c r="A25" s="18"/>
       <c r="B25" s="3" t="s">
         <v>56</v>
@@ -1894,7 +1978,7 @@
       </c>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:12">
       <c r="A26" s="18"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1905,8 +1989,15 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="20"/>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="L26" s="43">
+        <f>6844/96</f>
+        <v>71.291666666666671</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="19" t="s">
         <v>59</v>
       </c>
@@ -1938,8 +2029,10 @@
         <v>106.06104000000001</v>
       </c>
       <c r="J27" s="20"/>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="19"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1950,8 +2043,15 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
       <c r="J28" s="20"/>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="L28" s="44">
+        <f>F31/4800</f>
+        <v>7.2183477072557984</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="18" t="s">
         <v>64</v>
       </c>
@@ -1984,8 +2084,15 @@
         <v>0.21690040896000004</v>
       </c>
       <c r="J29" s="20"/>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="L29" s="44">
+        <f>F32/4800</f>
+        <v>5.0268804592187326</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="18"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1996,8 +2103,10 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="20"/>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="19" t="s">
         <v>75</v>
       </c>
@@ -2030,8 +2139,15 @@
         <v>5737.2830938337993</v>
       </c>
       <c r="J31" s="20"/>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="L31" s="43">
+        <f>71.29/7.22</f>
+        <v>9.8739612188365662</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="34" t="s">
         <v>76</v>
       </c>
@@ -2064,8 +2180,15 @@
         <v>268.02161632309924</v>
       </c>
       <c r="J32" s="20"/>
-    </row>
-    <row r="33" spans="1:10" s="20" customFormat="1">
+      <c r="K32" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="L32" s="43">
+        <f>71.29/5.03</f>
+        <v>14.172962226640159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="20" customFormat="1">
       <c r="A33" s="24"/>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
@@ -2076,7 +2199,7 @@
       <c r="H33" s="25"/>
       <c r="I33" s="25"/>
     </row>
-    <row r="34" spans="1:10" s="20" customFormat="1">
+    <row r="34" spans="1:11" s="20" customFormat="1">
       <c r="A34" s="40" t="s">
         <v>84</v>
       </c>
@@ -2089,42 +2212,43 @@
       <c r="H34" s="23"/>
       <c r="I34" s="23"/>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="49" t="s">
+    <row r="35" spans="1:11">
+      <c r="A35" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
       <c r="J35" s="20"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:11">
       <c r="A36" s="17" t="s">
         <v>77</v>
       </c>
       <c r="J36" s="20"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>79</v>
       </c>
       <c r="J37" s="20"/>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="K37" s="45"/>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="17" t="s">
         <v>72</v>
       </c>
       <c r="J38" s="20"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:11">
       <c r="J39" s="20"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:11">
       <c r="J40" s="20"/>
     </row>
   </sheetData>
@@ -2155,2158 +2279,2158 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="41" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="45">
-        <v>0</v>
-      </c>
-      <c r="B2" s="45">
-        <v>0</v>
-      </c>
-      <c r="C2" s="45">
-        <v>0</v>
-      </c>
-      <c r="D2" s="45" t="s">
+      <c r="A2" s="41">
+        <v>0</v>
+      </c>
+      <c r="B2" s="41">
+        <v>0</v>
+      </c>
+      <c r="C2" s="41">
+        <v>0</v>
+      </c>
+      <c r="D2" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="45">
+      <c r="A3" s="41">
         <v>96</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="42">
         <v>7400.08</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="41">
         <v>77.084166670000002</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="45">
+      <c r="A4" s="41">
         <v>192</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="41">
         <v>7956.16</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="41">
         <v>41.438333329999999</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="45">
+      <c r="A5" s="41">
         <v>288</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="41">
         <v>8512.24</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="41">
         <v>29.556388890000001</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="45">
+      <c r="A6" s="41">
         <v>384</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="42">
         <v>9068.32</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="41">
         <v>23.615416669999998</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="45">
+      <c r="A7" s="41">
         <v>480</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="42">
         <v>9624.4</v>
       </c>
-      <c r="C7" s="45">
+      <c r="C7" s="41">
         <v>20.05083333</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="45">
+      <c r="A8" s="41">
         <v>576</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="41">
         <v>10180.48</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="41">
         <v>17.674444439999998</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="45">
+      <c r="A9" s="41">
         <v>672</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="41">
         <v>10736.56</v>
       </c>
-      <c r="C9" s="45">
+      <c r="C9" s="41">
         <v>15.97702381</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="45">
+      <c r="A10" s="41">
         <v>768</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="42">
         <v>11292.64</v>
       </c>
-      <c r="C10" s="45">
+      <c r="C10" s="41">
         <v>14.703958330000001</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="45">
+      <c r="A11" s="41">
         <v>864</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="42">
         <v>11848.72</v>
       </c>
-      <c r="C11" s="45">
+      <c r="C11" s="41">
         <v>13.7137963</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="45">
+      <c r="A12" s="41">
         <v>960</v>
       </c>
-      <c r="B12" s="45">
+      <c r="B12" s="41">
         <v>12404.8</v>
       </c>
-      <c r="C12" s="45">
+      <c r="C12" s="41">
         <v>12.92166667</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="45">
+      <c r="A13" s="41">
         <v>1056</v>
       </c>
-      <c r="B13" s="45">
+      <c r="B13" s="41">
         <v>12960.88</v>
       </c>
-      <c r="C13" s="45">
+      <c r="C13" s="41">
         <v>12.273560610000001</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="45">
+      <c r="A14" s="41">
         <v>1152</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="42">
         <v>13516.96</v>
       </c>
-      <c r="C14" s="45">
+      <c r="C14" s="41">
         <v>11.733472219999999</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="45">
+      <c r="A15" s="41">
         <v>1248</v>
       </c>
-      <c r="B15" s="46">
+      <c r="B15" s="42">
         <v>14073.04</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C15" s="41">
         <v>11.27647436</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="45">
+      <c r="A16" s="41">
         <v>1344</v>
       </c>
-      <c r="B16" s="45">
+      <c r="B16" s="41">
         <v>14629.12</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C16" s="41">
         <v>10.884761900000001</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="45">
+      <c r="A17" s="41">
         <v>1440</v>
       </c>
-      <c r="B17" s="45">
+      <c r="B17" s="41">
         <v>15185.2</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="41">
         <v>10.545277779999999</v>
       </c>
-      <c r="D17" s="45" t="s">
+      <c r="D17" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="45">
+      <c r="A18" s="41">
         <v>1536</v>
       </c>
-      <c r="B18" s="46">
+      <c r="B18" s="42">
         <v>15741.28</v>
       </c>
-      <c r="C18" s="45">
+      <c r="C18" s="41">
         <v>10.24822917</v>
       </c>
-      <c r="D18" s="45" t="s">
+      <c r="D18" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="45">
+      <c r="A19" s="41">
         <v>1632</v>
       </c>
-      <c r="B19" s="46">
+      <c r="B19" s="42">
         <v>16297.36</v>
       </c>
-      <c r="C19" s="45">
+      <c r="C19" s="41">
         <v>9.9861274509999998</v>
       </c>
-      <c r="D19" s="45" t="s">
+      <c r="D19" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="45">
+      <c r="A20" s="41">
         <v>1728</v>
       </c>
-      <c r="B20" s="45">
+      <c r="B20" s="41">
         <v>16853.439999999999</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C20" s="41">
         <v>9.7531481479999993</v>
       </c>
-      <c r="D20" s="45" t="s">
+      <c r="D20" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="45">
+      <c r="A21" s="41">
         <v>1824</v>
       </c>
-      <c r="B21" s="45">
+      <c r="B21" s="41">
         <v>17409.52</v>
       </c>
-      <c r="C21" s="45">
+      <c r="C21" s="41">
         <v>9.5446929820000008</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D21" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="45">
+      <c r="A22" s="41">
         <v>1920</v>
       </c>
-      <c r="B22" s="46">
+      <c r="B22" s="42">
         <v>17965.599999999999</v>
       </c>
-      <c r="C22" s="45">
+      <c r="C22" s="41">
         <v>9.3570833330000003</v>
       </c>
-      <c r="D22" s="45" t="s">
+      <c r="D22" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="45">
+      <c r="A23" s="41">
         <v>2016</v>
       </c>
-      <c r="B23" s="46">
+      <c r="B23" s="42">
         <v>18521.68</v>
       </c>
-      <c r="C23" s="45">
+      <c r="C23" s="41">
         <v>9.1873412699999992</v>
       </c>
-      <c r="D23" s="45" t="s">
+      <c r="D23" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="45">
+      <c r="A24" s="41">
         <v>2112</v>
       </c>
-      <c r="B24" s="45">
+      <c r="B24" s="41">
         <v>19077.759999999998</v>
       </c>
-      <c r="C24" s="45">
+      <c r="C24" s="41">
         <v>9.0330303030000003</v>
       </c>
-      <c r="D24" s="45" t="s">
+      <c r="D24" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="45">
+      <c r="A25" s="41">
         <v>2208</v>
       </c>
-      <c r="B25" s="45">
+      <c r="B25" s="41">
         <v>19633.84</v>
       </c>
-      <c r="C25" s="45">
+      <c r="C25" s="41">
         <v>8.8921376809999995</v>
       </c>
-      <c r="D25" s="45" t="s">
+      <c r="D25" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="45">
+      <c r="A26" s="41">
         <v>2304</v>
       </c>
-      <c r="B26" s="46">
+      <c r="B26" s="42">
         <v>20189.919999999998</v>
       </c>
-      <c r="C26" s="45">
+      <c r="C26" s="41">
         <v>8.762986111</v>
       </c>
-      <c r="D26" s="45" t="s">
+      <c r="D26" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="45">
+      <c r="A27" s="41">
         <v>2400</v>
       </c>
-      <c r="B27" s="46">
+      <c r="B27" s="42">
         <v>20746</v>
       </c>
-      <c r="C27" s="45">
+      <c r="C27" s="41">
         <v>8.6441666670000004</v>
       </c>
-      <c r="D27" s="45" t="s">
+      <c r="D27" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="45">
+      <c r="A28" s="41">
         <v>2496</v>
       </c>
-      <c r="B28" s="45">
+      <c r="B28" s="41">
         <v>21302.080000000002</v>
       </c>
-      <c r="C28" s="45">
+      <c r="C28" s="41">
         <v>8.5344871789999992</v>
       </c>
-      <c r="D28" s="45" t="s">
+      <c r="D28" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="45">
+      <c r="A29" s="41">
         <v>2592</v>
       </c>
-      <c r="B29" s="45">
+      <c r="B29" s="41">
         <v>21858.16</v>
       </c>
-      <c r="C29" s="45">
+      <c r="C29" s="41">
         <v>8.4329320990000003</v>
       </c>
-      <c r="D29" s="45" t="s">
+      <c r="D29" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="45">
+      <c r="A30" s="41">
         <v>2688</v>
       </c>
-      <c r="B30" s="46">
+      <c r="B30" s="42">
         <v>22414.240000000002</v>
       </c>
-      <c r="C30" s="45">
+      <c r="C30" s="41">
         <v>8.3386309520000008</v>
       </c>
-      <c r="D30" s="45" t="s">
+      <c r="D30" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="45">
+      <c r="A31" s="41">
         <v>2784</v>
       </c>
-      <c r="B31" s="46">
+      <c r="B31" s="42">
         <v>22970.32</v>
       </c>
-      <c r="C31" s="45">
+      <c r="C31" s="41">
         <v>8.2508333329999992</v>
       </c>
-      <c r="D31" s="45" t="s">
+      <c r="D31" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="45">
+      <c r="A32" s="41">
         <v>2880</v>
       </c>
-      <c r="B32" s="45">
+      <c r="B32" s="41">
         <v>23526.400000000001</v>
       </c>
-      <c r="C32" s="45">
+      <c r="C32" s="41">
         <v>8.1688888889999998</v>
       </c>
-      <c r="D32" s="45" t="s">
+      <c r="D32" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="45">
+      <c r="A33" s="41">
         <v>2976</v>
       </c>
-      <c r="B33" s="45">
+      <c r="B33" s="41">
         <v>24082.48</v>
       </c>
-      <c r="C33" s="45">
+      <c r="C33" s="41">
         <v>8.0922311830000009</v>
       </c>
-      <c r="D33" s="45" t="s">
+      <c r="D33" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="45">
+      <c r="A34" s="41">
         <v>3072</v>
       </c>
-      <c r="B34" s="46">
+      <c r="B34" s="42">
         <v>24638.560000000001</v>
       </c>
-      <c r="C34" s="45">
+      <c r="C34" s="41">
         <v>8.0203645829999992</v>
       </c>
-      <c r="D34" s="45" t="s">
+      <c r="D34" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="45">
+      <c r="A35" s="41">
         <v>3168</v>
       </c>
-      <c r="B35" s="46">
+      <c r="B35" s="42">
         <v>25194.639999999999</v>
       </c>
-      <c r="C35" s="45">
+      <c r="C35" s="41">
         <v>7.952853535</v>
       </c>
-      <c r="D35" s="45" t="s">
+      <c r="D35" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="45">
+      <c r="A36" s="41">
         <v>3264</v>
       </c>
-      <c r="B36" s="45">
+      <c r="B36" s="41">
         <v>25750.720000000001</v>
       </c>
-      <c r="C36" s="45">
+      <c r="C36" s="41">
         <v>7.8893137250000001</v>
       </c>
-      <c r="D36" s="45" t="s">
+      <c r="D36" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="45">
+      <c r="A37" s="41">
         <v>3360</v>
       </c>
-      <c r="B37" s="45">
+      <c r="B37" s="41">
         <v>26306.799999999999</v>
       </c>
-      <c r="C37" s="45">
+      <c r="C37" s="41">
         <v>7.8294047620000002</v>
       </c>
-      <c r="D37" s="45" t="s">
+      <c r="D37" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="45">
+      <c r="A38" s="41">
         <v>3456</v>
       </c>
-      <c r="B38" s="46">
+      <c r="B38" s="42">
         <v>26862.880000000001</v>
       </c>
-      <c r="C38" s="45">
+      <c r="C38" s="41">
         <v>7.7728240739999999</v>
       </c>
-      <c r="D38" s="45" t="s">
+      <c r="D38" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="45">
+      <c r="A39" s="41">
         <v>3552</v>
       </c>
-      <c r="B39" s="46">
+      <c r="B39" s="42">
         <v>27418.959999999999</v>
       </c>
-      <c r="C39" s="45">
+      <c r="C39" s="41">
         <v>7.7193018020000004</v>
       </c>
-      <c r="D39" s="45" t="s">
+      <c r="D39" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="45">
+      <c r="A40" s="41">
         <v>3648</v>
       </c>
-      <c r="B40" s="45">
+      <c r="B40" s="41">
         <v>27975.040000000001</v>
       </c>
-      <c r="C40" s="45">
+      <c r="C40" s="41">
         <v>7.6685964909999997</v>
       </c>
-      <c r="D40" s="45" t="s">
+      <c r="D40" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="45">
+      <c r="A41" s="41">
         <v>3744</v>
       </c>
-      <c r="B41" s="45">
+      <c r="B41" s="41">
         <v>28531.119999999999</v>
       </c>
-      <c r="C41" s="45">
+      <c r="C41" s="41">
         <v>7.6204914529999996</v>
       </c>
-      <c r="D41" s="45" t="s">
+      <c r="D41" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="45">
+      <c r="A42" s="41">
         <v>3840</v>
       </c>
-      <c r="B42" s="46">
+      <c r="B42" s="42">
         <v>29087.200000000001</v>
       </c>
-      <c r="C42" s="45">
+      <c r="C42" s="41">
         <v>7.5747916670000004</v>
       </c>
-      <c r="D42" s="45" t="s">
+      <c r="D42" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="45">
+      <c r="A43" s="41">
         <v>3936</v>
       </c>
-      <c r="B43" s="46">
+      <c r="B43" s="42">
         <v>29643.279999999999</v>
       </c>
-      <c r="C43" s="45">
+      <c r="C43" s="41">
         <v>7.531321138</v>
       </c>
-      <c r="D43" s="45" t="s">
+      <c r="D43" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="45">
+      <c r="A44" s="41">
         <v>4032</v>
       </c>
-      <c r="B44" s="45">
+      <c r="B44" s="41">
         <v>30199.360000000001</v>
       </c>
-      <c r="C44" s="45">
+      <c r="C44" s="41">
         <v>7.4899206349999998</v>
       </c>
-      <c r="D44" s="45" t="s">
+      <c r="D44" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="45">
+      <c r="A45" s="41">
         <v>4128</v>
       </c>
-      <c r="B45" s="45">
+      <c r="B45" s="41">
         <v>30755.439999999999</v>
       </c>
-      <c r="C45" s="45">
+      <c r="C45" s="41">
         <v>7.4504457359999998</v>
       </c>
-      <c r="D45" s="45" t="s">
+      <c r="D45" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="45">
+      <c r="A46" s="41">
         <v>4224</v>
       </c>
-      <c r="B46" s="46">
+      <c r="B46" s="42">
         <v>31311.52</v>
       </c>
-      <c r="C46" s="45">
+      <c r="C46" s="41">
         <v>7.4127651520000004</v>
       </c>
-      <c r="D46" s="45" t="s">
+      <c r="D46" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="45">
+      <c r="A47" s="41">
         <v>4320</v>
       </c>
-      <c r="B47" s="46">
+      <c r="B47" s="42">
         <v>31867.599999999999</v>
       </c>
-      <c r="C47" s="45">
+      <c r="C47" s="41">
         <v>7.376759259</v>
       </c>
-      <c r="D47" s="45" t="s">
+      <c r="D47" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="45">
+      <c r="A48" s="41">
         <v>4416</v>
       </c>
-      <c r="B48" s="45">
+      <c r="B48" s="41">
         <v>32423.68</v>
       </c>
-      <c r="C48" s="45">
+      <c r="C48" s="41">
         <v>7.342318841</v>
       </c>
-      <c r="D48" s="45" t="s">
+      <c r="D48" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="45">
+      <c r="A49" s="41">
         <v>4512</v>
       </c>
-      <c r="B49" s="45">
+      <c r="B49" s="41">
         <v>32979.760000000002</v>
       </c>
-      <c r="C49" s="45">
+      <c r="C49" s="41">
         <v>7.3093439719999997</v>
       </c>
-      <c r="D49" s="45" t="s">
+      <c r="D49" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="45">
+      <c r="A50" s="41">
         <v>4608</v>
       </c>
-      <c r="B50" s="46">
+      <c r="B50" s="42">
         <v>33535.839999999997</v>
       </c>
-      <c r="C50" s="45">
+      <c r="C50" s="41">
         <v>7.2777430560000003</v>
       </c>
-      <c r="D50" s="45" t="s">
+      <c r="D50" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="45">
+      <c r="A51" s="41">
         <v>4704</v>
       </c>
-      <c r="B51" s="46">
+      <c r="B51" s="42">
         <v>34091.919999999998</v>
       </c>
-      <c r="C51" s="45">
+      <c r="C51" s="41">
         <v>7.2474319730000003</v>
       </c>
-      <c r="D51" s="45" t="s">
+      <c r="D51" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="45">
+      <c r="A52" s="41">
         <v>4800</v>
       </c>
-      <c r="B52" s="45">
+      <c r="B52" s="41">
         <v>34648</v>
       </c>
-      <c r="C52" s="45">
+      <c r="C52" s="41">
         <v>7.2183333330000004</v>
       </c>
-      <c r="D52" s="45" t="s">
+      <c r="D52" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="45">
-        <v>0</v>
-      </c>
-      <c r="B53" s="45">
-        <v>0</v>
-      </c>
-      <c r="C53" s="45" t="e">
+      <c r="A53" s="41">
+        <v>0</v>
+      </c>
+      <c r="B53" s="41">
+        <v>0</v>
+      </c>
+      <c r="C53" s="41" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="D53" s="45" t="s">
+      <c r="D53" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="45">
+      <c r="A54" s="41">
         <v>96</v>
       </c>
-      <c r="B54" s="45">
+      <c r="B54" s="41">
         <v>7189.7</v>
       </c>
-      <c r="C54" s="45">
+      <c r="C54" s="41">
         <v>74.892708330000005</v>
       </c>
-      <c r="D54" s="45" t="s">
+      <c r="D54" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="45">
+      <c r="A55" s="41">
         <v>192</v>
       </c>
-      <c r="B55" s="45">
+      <c r="B55" s="41">
         <v>7535.4</v>
       </c>
-      <c r="C55" s="45">
+      <c r="C55" s="41">
         <v>39.246875000000003</v>
       </c>
-      <c r="D55" s="45" t="s">
+      <c r="D55" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="45">
+      <c r="A56" s="41">
         <v>288</v>
       </c>
-      <c r="B56" s="45">
+      <c r="B56" s="41">
         <v>7881.1</v>
       </c>
-      <c r="C56" s="45">
+      <c r="C56" s="41">
         <v>27.364930560000001</v>
       </c>
-      <c r="D56" s="45" t="s">
+      <c r="D56" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="45">
+      <c r="A57" s="41">
         <v>384</v>
       </c>
-      <c r="B57" s="45">
+      <c r="B57" s="41">
         <v>8226.7999999999993</v>
       </c>
-      <c r="C57" s="45">
+      <c r="C57" s="41">
         <v>21.423958330000001</v>
       </c>
-      <c r="D57" s="45" t="s">
+      <c r="D57" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="45">
+      <c r="A58" s="41">
         <v>480</v>
       </c>
-      <c r="B58" s="45">
+      <c r="B58" s="41">
         <v>8572.5</v>
       </c>
-      <c r="C58" s="45">
+      <c r="C58" s="41">
         <v>17.859375</v>
       </c>
-      <c r="D58" s="45" t="s">
+      <c r="D58" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="45">
+      <c r="A59" s="41">
         <v>576</v>
       </c>
-      <c r="B59" s="45">
+      <c r="B59" s="41">
         <v>8918.2000000000007</v>
       </c>
-      <c r="C59" s="45">
+      <c r="C59" s="41">
         <v>15.482986110000001</v>
       </c>
-      <c r="D59" s="45" t="s">
+      <c r="D59" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="45">
+      <c r="A60" s="41">
         <v>672</v>
       </c>
-      <c r="B60" s="45">
+      <c r="B60" s="41">
         <v>9263.9</v>
       </c>
-      <c r="C60" s="45">
+      <c r="C60" s="41">
         <v>13.785565480000001</v>
       </c>
-      <c r="D60" s="45" t="s">
+      <c r="D60" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="45">
+      <c r="A61" s="41">
         <v>768</v>
       </c>
-      <c r="B61" s="45">
+      <c r="B61" s="41">
         <v>9609.6</v>
       </c>
-      <c r="C61" s="45">
+      <c r="C61" s="41">
         <v>12.512499999999999</v>
       </c>
-      <c r="D61" s="45" t="s">
+      <c r="D61" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="45">
+      <c r="A62" s="41">
         <v>864</v>
       </c>
-      <c r="B62" s="45">
+      <c r="B62" s="41">
         <v>9955.2999999999993</v>
       </c>
-      <c r="C62" s="45">
+      <c r="C62" s="41">
         <v>11.52233796</v>
       </c>
-      <c r="D62" s="45" t="s">
+      <c r="D62" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="45">
+      <c r="A63" s="41">
         <v>960</v>
       </c>
-      <c r="B63" s="45">
+      <c r="B63" s="41">
         <v>10301</v>
       </c>
-      <c r="C63" s="45">
+      <c r="C63" s="41">
         <v>10.73020833</v>
       </c>
-      <c r="D63" s="45" t="s">
+      <c r="D63" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="45">
+      <c r="A64" s="41">
         <v>1056</v>
       </c>
-      <c r="B64" s="45">
+      <c r="B64" s="41">
         <v>10646.7</v>
       </c>
-      <c r="C64" s="45">
+      <c r="C64" s="41">
         <v>10.08210227</v>
       </c>
-      <c r="D64" s="45" t="s">
+      <c r="D64" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="45">
+      <c r="A65" s="41">
         <v>1152</v>
       </c>
-      <c r="B65" s="45">
+      <c r="B65" s="41">
         <v>10992.4</v>
       </c>
-      <c r="C65" s="45">
+      <c r="C65" s="41">
         <v>9.5420138889999997</v>
       </c>
-      <c r="D65" s="45" t="s">
+      <c r="D65" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="45">
+      <c r="A66" s="41">
         <v>1248</v>
       </c>
-      <c r="B66" s="45">
+      <c r="B66" s="41">
         <v>11338.1</v>
       </c>
-      <c r="C66" s="45">
+      <c r="C66" s="41">
         <v>9.0850160259999999</v>
       </c>
-      <c r="D66" s="45" t="s">
+      <c r="D66" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="45">
+      <c r="A67" s="41">
         <v>1344</v>
       </c>
-      <c r="B67" s="45">
+      <c r="B67" s="41">
         <v>11683.8</v>
       </c>
-      <c r="C67" s="45">
+      <c r="C67" s="41">
         <v>8.6933035709999995</v>
       </c>
-      <c r="D67" s="45" t="s">
+      <c r="D67" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="45">
+      <c r="A68" s="41">
         <v>1440</v>
       </c>
-      <c r="B68" s="45">
+      <c r="B68" s="41">
         <v>12029.5</v>
       </c>
-      <c r="C68" s="45">
+      <c r="C68" s="41">
         <v>8.3538194440000009</v>
       </c>
-      <c r="D68" s="45" t="s">
+      <c r="D68" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="45">
+      <c r="A69" s="41">
         <v>1536</v>
       </c>
-      <c r="B69" s="45">
+      <c r="B69" s="41">
         <v>12375.2</v>
       </c>
-      <c r="C69" s="45">
+      <c r="C69" s="41">
         <v>8.0567708329999999</v>
       </c>
-      <c r="D69" s="45" t="s">
+      <c r="D69" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="45">
+      <c r="A70" s="41">
         <v>1632</v>
       </c>
-      <c r="B70" s="45">
+      <c r="B70" s="41">
         <v>12720.9</v>
       </c>
-      <c r="C70" s="45">
+      <c r="C70" s="41">
         <v>7.7946691179999998</v>
       </c>
-      <c r="D70" s="45" t="s">
+      <c r="D70" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="45">
+      <c r="A71" s="41">
         <v>1728</v>
       </c>
-      <c r="B71" s="45">
+      <c r="B71" s="41">
         <v>13066.6</v>
       </c>
-      <c r="C71" s="45">
+      <c r="C71" s="41">
         <v>7.5616898150000003</v>
       </c>
-      <c r="D71" s="45" t="s">
+      <c r="D71" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="45">
+      <c r="A72" s="41">
         <v>1824</v>
       </c>
-      <c r="B72" s="45">
+      <c r="B72" s="41">
         <v>13412.3</v>
       </c>
-      <c r="C72" s="45">
+      <c r="C72" s="41">
         <v>7.353234649</v>
       </c>
-      <c r="D72" s="45" t="s">
+      <c r="D72" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="45">
+      <c r="A73" s="41">
         <v>1920</v>
       </c>
-      <c r="B73" s="45">
+      <c r="B73" s="41">
         <v>13758</v>
       </c>
-      <c r="C73" s="45">
+      <c r="C73" s="41">
         <v>7.1656250000000004</v>
       </c>
-      <c r="D73" s="45" t="s">
+      <c r="D73" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="45">
+      <c r="A74" s="41">
         <v>2016</v>
       </c>
-      <c r="B74" s="45">
+      <c r="B74" s="41">
         <v>14103.7</v>
       </c>
-      <c r="C74" s="45">
+      <c r="C74" s="41">
         <v>6.9958829370000002</v>
       </c>
-      <c r="D74" s="45" t="s">
+      <c r="D74" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="45">
+      <c r="A75" s="41">
         <v>2112</v>
       </c>
-      <c r="B75" s="45">
+      <c r="B75" s="41">
         <v>14449.4</v>
       </c>
-      <c r="C75" s="45">
+      <c r="C75" s="41">
         <v>6.8415719700000004</v>
       </c>
-      <c r="D75" s="45" t="s">
+      <c r="D75" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="45">
+      <c r="A76" s="41">
         <v>2208</v>
       </c>
-      <c r="B76" s="45">
+      <c r="B76" s="41">
         <v>14795.1</v>
       </c>
-      <c r="C76" s="45">
+      <c r="C76" s="41">
         <v>6.7006793480000004</v>
       </c>
-      <c r="D76" s="45" t="s">
+      <c r="D76" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="45">
+      <c r="A77" s="41">
         <v>2304</v>
       </c>
-      <c r="B77" s="45">
+      <c r="B77" s="41">
         <v>15140.8</v>
       </c>
-      <c r="C77" s="45">
+      <c r="C77" s="41">
         <v>6.5715277780000001</v>
       </c>
-      <c r="D77" s="45" t="s">
+      <c r="D77" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="45">
+      <c r="A78" s="41">
         <v>2400</v>
       </c>
-      <c r="B78" s="45">
+      <c r="B78" s="41">
         <v>15486.5</v>
       </c>
-      <c r="C78" s="45">
+      <c r="C78" s="41">
         <v>6.4527083330000004</v>
       </c>
-      <c r="D78" s="45" t="s">
+      <c r="D78" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="45">
+      <c r="A79" s="41">
         <v>2496</v>
       </c>
-      <c r="B79" s="45">
+      <c r="B79" s="41">
         <v>15832.2</v>
       </c>
-      <c r="C79" s="45">
+      <c r="C79" s="41">
         <v>6.3430288460000002</v>
       </c>
-      <c r="D79" s="45" t="s">
+      <c r="D79" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="45">
+      <c r="A80" s="41">
         <v>2592</v>
       </c>
-      <c r="B80" s="45">
+      <c r="B80" s="41">
         <v>16177.9</v>
       </c>
-      <c r="C80" s="45">
+      <c r="C80" s="41">
         <v>6.2414737650000003</v>
       </c>
-      <c r="D80" s="45" t="s">
+      <c r="D80" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="45">
+      <c r="A81" s="41">
         <v>2688</v>
       </c>
-      <c r="B81" s="45">
+      <c r="B81" s="41">
         <v>16523.599999999999</v>
       </c>
-      <c r="C81" s="45">
+      <c r="C81" s="41">
         <v>6.147172619</v>
       </c>
-      <c r="D81" s="45" t="s">
+      <c r="D81" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="45">
+      <c r="A82" s="41">
         <v>2784</v>
       </c>
-      <c r="B82" s="45">
+      <c r="B82" s="41">
         <v>16869.3</v>
       </c>
-      <c r="C82" s="45">
+      <c r="C82" s="41">
         <v>6.0593750000000002</v>
       </c>
-      <c r="D82" s="45" t="s">
+      <c r="D82" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="45">
+      <c r="A83" s="41">
         <v>2880</v>
       </c>
-      <c r="B83" s="45">
+      <c r="B83" s="41">
         <v>17215</v>
       </c>
-      <c r="C83" s="45">
+      <c r="C83" s="41">
         <v>5.9774305559999998</v>
       </c>
-      <c r="D83" s="45" t="s">
+      <c r="D83" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="45">
+      <c r="A84" s="41">
         <v>2976</v>
       </c>
-      <c r="B84" s="45">
+      <c r="B84" s="41">
         <v>17560.7</v>
       </c>
-      <c r="C84" s="45">
+      <c r="C84" s="41">
         <v>5.900772849</v>
       </c>
-      <c r="D84" s="45" t="s">
+      <c r="D84" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="45">
+      <c r="A85" s="41">
         <v>3072</v>
       </c>
-      <c r="B85" s="45">
+      <c r="B85" s="41">
         <v>17906.400000000001</v>
       </c>
-      <c r="C85" s="45">
+      <c r="C85" s="41">
         <v>5.8289062500000002</v>
       </c>
-      <c r="D85" s="45" t="s">
+      <c r="D85" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="45">
+      <c r="A86" s="41">
         <v>3168</v>
       </c>
-      <c r="B86" s="45">
+      <c r="B86" s="41">
         <v>18252.099999999999</v>
       </c>
-      <c r="C86" s="45">
+      <c r="C86" s="41">
         <v>5.7613952020000001</v>
       </c>
-      <c r="D86" s="45" t="s">
+      <c r="D86" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="45">
+      <c r="A87" s="41">
         <v>3264</v>
       </c>
-      <c r="B87" s="45">
+      <c r="B87" s="41">
         <v>18597.8</v>
       </c>
-      <c r="C87" s="45">
+      <c r="C87" s="41">
         <v>5.6978553920000001</v>
       </c>
-      <c r="D87" s="45" t="s">
+      <c r="D87" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="45">
+      <c r="A88" s="41">
         <v>3360</v>
       </c>
-      <c r="B88" s="45">
+      <c r="B88" s="41">
         <v>18943.5</v>
       </c>
-      <c r="C88" s="45">
+      <c r="C88" s="41">
         <v>5.6379464290000003</v>
       </c>
-      <c r="D88" s="45" t="s">
+      <c r="D88" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="45">
+      <c r="A89" s="41">
         <v>3456</v>
       </c>
-      <c r="B89" s="45">
+      <c r="B89" s="41">
         <v>19289.2</v>
       </c>
-      <c r="C89" s="45">
+      <c r="C89" s="41">
         <v>5.5813657409999999</v>
       </c>
-      <c r="D89" s="45" t="s">
+      <c r="D89" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="45">
+      <c r="A90" s="41">
         <v>3552</v>
       </c>
-      <c r="B90" s="45">
+      <c r="B90" s="41">
         <v>19634.900000000001</v>
       </c>
-      <c r="C90" s="45">
+      <c r="C90" s="41">
         <v>5.5278434680000004</v>
       </c>
-      <c r="D90" s="45" t="s">
+      <c r="D90" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="45">
+      <c r="A91" s="41">
         <v>3648</v>
       </c>
-      <c r="B91" s="45">
+      <c r="B91" s="41">
         <v>19980.599999999999</v>
       </c>
-      <c r="C91" s="45">
+      <c r="C91" s="41">
         <v>5.4771381579999998</v>
       </c>
-      <c r="D91" s="45" t="s">
+      <c r="D91" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="45">
+      <c r="A92" s="41">
         <v>3744</v>
       </c>
-      <c r="B92" s="45">
+      <c r="B92" s="41">
         <v>20326.3</v>
       </c>
-      <c r="C92" s="45">
+      <c r="C92" s="41">
         <v>5.4290331199999997</v>
       </c>
-      <c r="D92" s="45" t="s">
+      <c r="D92" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="45">
+      <c r="A93" s="41">
         <v>3840</v>
       </c>
-      <c r="B93" s="45">
+      <c r="B93" s="41">
         <v>20672</v>
       </c>
-      <c r="C93" s="45">
+      <c r="C93" s="41">
         <v>5.3833333330000004</v>
       </c>
-      <c r="D93" s="45" t="s">
+      <c r="D93" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="45">
+      <c r="A94" s="41">
         <v>3936</v>
       </c>
-      <c r="B94" s="45">
+      <c r="B94" s="41">
         <v>21017.7</v>
       </c>
-      <c r="C94" s="45">
+      <c r="C94" s="41">
         <v>5.3398628050000001</v>
       </c>
-      <c r="D94" s="45" t="s">
+      <c r="D94" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="45">
+      <c r="A95" s="41">
         <v>4032</v>
       </c>
-      <c r="B95" s="45">
+      <c r="B95" s="41">
         <v>21363.4</v>
       </c>
-      <c r="C95" s="45">
+      <c r="C95" s="41">
         <v>5.2984623019999999</v>
       </c>
-      <c r="D95" s="45" t="s">
+      <c r="D95" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="45">
+      <c r="A96" s="41">
         <v>4128</v>
       </c>
-      <c r="B96" s="45">
+      <c r="B96" s="41">
         <v>21709.1</v>
       </c>
-      <c r="C96" s="45">
+      <c r="C96" s="41">
         <v>5.2589874029999999</v>
       </c>
-      <c r="D96" s="45" t="s">
+      <c r="D96" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="45">
+      <c r="A97" s="41">
         <v>4224</v>
       </c>
-      <c r="B97" s="45">
+      <c r="B97" s="41">
         <v>22054.799999999999</v>
       </c>
-      <c r="C97" s="45">
+      <c r="C97" s="41">
         <v>5.2213068180000004</v>
       </c>
-      <c r="D97" s="45" t="s">
+      <c r="D97" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="45">
+      <c r="A98" s="41">
         <v>4320</v>
       </c>
-      <c r="B98" s="45">
+      <c r="B98" s="41">
         <v>22400.5</v>
       </c>
-      <c r="C98" s="45">
+      <c r="C98" s="41">
         <v>5.185300926</v>
       </c>
-      <c r="D98" s="45" t="s">
+      <c r="D98" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="45">
+      <c r="A99" s="41">
         <v>4416</v>
       </c>
-      <c r="B99" s="45">
+      <c r="B99" s="41">
         <v>22746.2</v>
       </c>
-      <c r="C99" s="45">
+      <c r="C99" s="41">
         <v>5.150860507</v>
       </c>
-      <c r="D99" s="45" t="s">
+      <c r="D99" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="45">
+      <c r="A100" s="41">
         <v>4512</v>
       </c>
-      <c r="B100" s="45">
+      <c r="B100" s="41">
         <v>23091.9</v>
       </c>
-      <c r="C100" s="45">
+      <c r="C100" s="41">
         <v>5.1178856379999997</v>
       </c>
-      <c r="D100" s="45" t="s">
+      <c r="D100" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="45">
+      <c r="A101" s="41">
         <v>4608</v>
       </c>
-      <c r="B101" s="45">
+      <c r="B101" s="41">
         <v>23437.599999999999</v>
       </c>
-      <c r="C101" s="45">
+      <c r="C101" s="41">
         <v>5.0862847220000003</v>
       </c>
-      <c r="D101" s="45" t="s">
+      <c r="D101" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="45">
+      <c r="A102" s="41">
         <v>4704</v>
       </c>
-      <c r="B102" s="45">
+      <c r="B102" s="41">
         <v>23783.3</v>
       </c>
-      <c r="C102" s="45">
+      <c r="C102" s="41">
         <v>5.0559736390000003</v>
       </c>
-      <c r="D102" s="45" t="s">
+      <c r="D102" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="45">
+      <c r="A103" s="41">
         <v>4800</v>
       </c>
-      <c r="B103" s="45">
+      <c r="B103" s="41">
         <v>24129</v>
       </c>
-      <c r="C103" s="45">
+      <c r="C103" s="41">
         <v>5.0268750000000004</v>
       </c>
-      <c r="D103" s="45" t="s">
+      <c r="D103" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="45">
-        <v>0</v>
-      </c>
-      <c r="B104" s="45">
-        <v>0</v>
-      </c>
-      <c r="C104" s="45">
-        <v>0</v>
-      </c>
-      <c r="D104" s="45" t="s">
+      <c r="A104" s="41">
+        <v>0</v>
+      </c>
+      <c r="B104" s="41">
+        <v>0</v>
+      </c>
+      <c r="C104" s="41">
+        <v>0</v>
+      </c>
+      <c r="D104" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="45">
+      <c r="A105" s="41">
         <v>96</v>
       </c>
-      <c r="B105" s="45">
+      <c r="B105" s="41">
         <v>6844</v>
       </c>
-      <c r="C105" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D105" s="45" t="s">
+      <c r="C105" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D105" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="45">
+      <c r="A106" s="41">
         <v>192</v>
       </c>
-      <c r="B106" s="45">
+      <c r="B106" s="41">
         <v>13688</v>
       </c>
-      <c r="C106" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D106" s="45" t="s">
+      <c r="C106" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D106" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="45">
+      <c r="A107" s="41">
         <v>288</v>
       </c>
-      <c r="B107" s="45">
+      <c r="B107" s="41">
         <v>20532</v>
       </c>
-      <c r="C107" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D107" s="45" t="s">
+      <c r="C107" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D107" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:4">
-      <c r="A108" s="45">
+      <c r="A108" s="41">
         <v>384</v>
       </c>
-      <c r="B108" s="45">
+      <c r="B108" s="41">
         <v>27376</v>
       </c>
-      <c r="C108" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D108" s="45" t="s">
+      <c r="C108" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D108" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" s="45">
+      <c r="A109" s="41">
         <v>480</v>
       </c>
-      <c r="B109" s="45">
+      <c r="B109" s="41">
         <v>34220</v>
       </c>
-      <c r="C109" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D109" s="45" t="s">
+      <c r="C109" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D109" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:4">
-      <c r="A110" s="45">
+      <c r="A110" s="41">
         <v>576</v>
       </c>
-      <c r="B110" s="45">
+      <c r="B110" s="41">
         <v>41064</v>
       </c>
-      <c r="C110" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D110" s="45" t="s">
+      <c r="C110" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D110" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:4">
-      <c r="A111" s="45">
+      <c r="A111" s="41">
         <v>672</v>
       </c>
-      <c r="B111" s="45">
+      <c r="B111" s="41">
         <v>47908</v>
       </c>
-      <c r="C111" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D111" s="45" t="s">
+      <c r="C111" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D111" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" s="45">
+      <c r="A112" s="41">
         <v>768</v>
       </c>
-      <c r="B112" s="45">
+      <c r="B112" s="41">
         <v>54752</v>
       </c>
-      <c r="C112" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D112" s="45" t="s">
+      <c r="C112" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D112" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:4">
-      <c r="A113" s="45">
+      <c r="A113" s="41">
         <v>864</v>
       </c>
-      <c r="B113" s="45">
+      <c r="B113" s="41">
         <v>61596</v>
       </c>
-      <c r="C113" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D113" s="45" t="s">
+      <c r="C113" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D113" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:4">
-      <c r="A114" s="45">
+      <c r="A114" s="41">
         <v>960</v>
       </c>
-      <c r="B114" s="45">
+      <c r="B114" s="41">
         <v>68440</v>
       </c>
-      <c r="C114" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D114" s="45" t="s">
+      <c r="C114" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D114" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:4">
-      <c r="A115" s="45">
+      <c r="A115" s="41">
         <v>1056</v>
       </c>
-      <c r="B115" s="45">
+      <c r="B115" s="41">
         <v>75284</v>
       </c>
-      <c r="C115" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D115" s="45" t="s">
+      <c r="C115" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D115" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:4">
-      <c r="A116" s="45">
+      <c r="A116" s="41">
         <v>1152</v>
       </c>
-      <c r="B116" s="45">
+      <c r="B116" s="41">
         <v>82128</v>
       </c>
-      <c r="C116" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D116" s="45" t="s">
+      <c r="C116" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D116" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:4">
-      <c r="A117" s="45">
+      <c r="A117" s="41">
         <v>1248</v>
       </c>
-      <c r="B117" s="45">
+      <c r="B117" s="41">
         <v>88972</v>
       </c>
-      <c r="C117" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D117" s="45" t="s">
+      <c r="C117" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D117" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" s="45">
+      <c r="A118" s="41">
         <v>1344</v>
       </c>
-      <c r="B118" s="45">
+      <c r="B118" s="41">
         <v>95816</v>
       </c>
-      <c r="C118" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D118" s="45" t="s">
+      <c r="C118" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D118" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:4">
-      <c r="A119" s="45">
+      <c r="A119" s="41">
         <v>1440</v>
       </c>
-      <c r="B119" s="45">
+      <c r="B119" s="41">
         <v>102660</v>
       </c>
-      <c r="C119" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D119" s="45" t="s">
+      <c r="C119" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D119" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="45">
+      <c r="A120" s="41">
         <v>1536</v>
       </c>
-      <c r="B120" s="45">
+      <c r="B120" s="41">
         <v>109504</v>
       </c>
-      <c r="C120" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D120" s="45" t="s">
+      <c r="C120" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D120" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:4">
-      <c r="A121" s="45">
+      <c r="A121" s="41">
         <v>1632</v>
       </c>
-      <c r="B121" s="45">
+      <c r="B121" s="41">
         <v>116348</v>
       </c>
-      <c r="C121" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D121" s="45" t="s">
+      <c r="C121" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D121" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:4">
-      <c r="A122" s="45">
+      <c r="A122" s="41">
         <v>1728</v>
       </c>
-      <c r="B122" s="45">
+      <c r="B122" s="41">
         <v>123192</v>
       </c>
-      <c r="C122" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D122" s="45" t="s">
+      <c r="C122" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D122" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:4">
-      <c r="A123" s="45">
+      <c r="A123" s="41">
         <v>1824</v>
       </c>
-      <c r="B123" s="45">
+      <c r="B123" s="41">
         <v>130036</v>
       </c>
-      <c r="C123" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D123" s="45" t="s">
+      <c r="C123" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D123" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:4">
-      <c r="A124" s="45">
+      <c r="A124" s="41">
         <v>1920</v>
       </c>
-      <c r="B124" s="45">
+      <c r="B124" s="41">
         <v>136880</v>
       </c>
-      <c r="C124" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D124" s="45" t="s">
+      <c r="C124" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D124" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:4">
-      <c r="A125" s="45">
+      <c r="A125" s="41">
         <v>2016</v>
       </c>
-      <c r="B125" s="45">
+      <c r="B125" s="41">
         <v>143724</v>
       </c>
-      <c r="C125" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D125" s="45" t="s">
+      <c r="C125" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D125" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:4">
-      <c r="A126" s="45">
+      <c r="A126" s="41">
         <v>2112</v>
       </c>
-      <c r="B126" s="45">
+      <c r="B126" s="41">
         <v>150568</v>
       </c>
-      <c r="C126" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D126" s="45" t="s">
+      <c r="C126" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D126" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:4">
-      <c r="A127" s="45">
+      <c r="A127" s="41">
         <v>2208</v>
       </c>
-      <c r="B127" s="45">
+      <c r="B127" s="41">
         <v>157412</v>
       </c>
-      <c r="C127" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D127" s="45" t="s">
+      <c r="C127" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D127" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:4">
-      <c r="A128" s="45">
+      <c r="A128" s="41">
         <v>2304</v>
       </c>
-      <c r="B128" s="45">
+      <c r="B128" s="41">
         <v>164256</v>
       </c>
-      <c r="C128" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D128" s="45" t="s">
+      <c r="C128" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D128" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:4">
-      <c r="A129" s="45">
+      <c r="A129" s="41">
         <v>2400</v>
       </c>
-      <c r="B129" s="45">
+      <c r="B129" s="41">
         <v>171100</v>
       </c>
-      <c r="C129" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D129" s="45" t="s">
+      <c r="C129" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D129" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:4">
-      <c r="A130" s="45">
+      <c r="A130" s="41">
         <v>2496</v>
       </c>
-      <c r="B130" s="45">
+      <c r="B130" s="41">
         <v>177944</v>
       </c>
-      <c r="C130" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D130" s="45" t="s">
+      <c r="C130" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D130" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:4">
-      <c r="A131" s="45">
+      <c r="A131" s="41">
         <v>2592</v>
       </c>
-      <c r="B131" s="45">
+      <c r="B131" s="41">
         <v>184788</v>
       </c>
-      <c r="C131" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D131" s="45" t="s">
+      <c r="C131" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D131" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:4">
-      <c r="A132" s="45">
+      <c r="A132" s="41">
         <v>2688</v>
       </c>
-      <c r="B132" s="45">
+      <c r="B132" s="41">
         <v>191632</v>
       </c>
-      <c r="C132" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D132" s="45" t="s">
+      <c r="C132" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D132" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:4">
-      <c r="A133" s="45">
+      <c r="A133" s="41">
         <v>2784</v>
       </c>
-      <c r="B133" s="45">
+      <c r="B133" s="41">
         <v>198476</v>
       </c>
-      <c r="C133" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D133" s="45" t="s">
+      <c r="C133" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D133" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:4">
-      <c r="A134" s="45">
+      <c r="A134" s="41">
         <v>2880</v>
       </c>
-      <c r="B134" s="45">
+      <c r="B134" s="41">
         <v>205320</v>
       </c>
-      <c r="C134" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D134" s="45" t="s">
+      <c r="C134" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D134" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:4">
-      <c r="A135" s="45">
+      <c r="A135" s="41">
         <v>2976</v>
       </c>
-      <c r="B135" s="45">
+      <c r="B135" s="41">
         <v>212164</v>
       </c>
-      <c r="C135" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D135" s="45" t="s">
+      <c r="C135" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D135" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:4">
-      <c r="A136" s="45">
+      <c r="A136" s="41">
         <v>3072</v>
       </c>
-      <c r="B136" s="45">
+      <c r="B136" s="41">
         <v>219008</v>
       </c>
-      <c r="C136" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D136" s="45" t="s">
+      <c r="C136" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D136" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:4">
-      <c r="A137" s="45">
+      <c r="A137" s="41">
         <v>3168</v>
       </c>
-      <c r="B137" s="45">
+      <c r="B137" s="41">
         <v>225852</v>
       </c>
-      <c r="C137" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D137" s="45" t="s">
+      <c r="C137" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D137" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:4">
-      <c r="A138" s="45">
+      <c r="A138" s="41">
         <v>3264</v>
       </c>
-      <c r="B138" s="45">
+      <c r="B138" s="41">
         <v>232696</v>
       </c>
-      <c r="C138" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D138" s="45" t="s">
+      <c r="C138" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D138" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:4">
-      <c r="A139" s="45">
+      <c r="A139" s="41">
         <v>3360</v>
       </c>
-      <c r="B139" s="45">
+      <c r="B139" s="41">
         <v>239540</v>
       </c>
-      <c r="C139" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D139" s="45" t="s">
+      <c r="C139" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D139" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:4">
-      <c r="A140" s="45">
+      <c r="A140" s="41">
         <v>3456</v>
       </c>
-      <c r="B140" s="45">
+      <c r="B140" s="41">
         <v>246384</v>
       </c>
-      <c r="C140" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D140" s="45" t="s">
+      <c r="C140" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D140" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:4">
-      <c r="A141" s="45">
+      <c r="A141" s="41">
         <v>3552</v>
       </c>
-      <c r="B141" s="45">
+      <c r="B141" s="41">
         <v>253228</v>
       </c>
-      <c r="C141" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D141" s="45" t="s">
+      <c r="C141" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D141" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:4">
-      <c r="A142" s="45">
+      <c r="A142" s="41">
         <v>3648</v>
       </c>
-      <c r="B142" s="45">
+      <c r="B142" s="41">
         <v>260072</v>
       </c>
-      <c r="C142" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D142" s="45" t="s">
+      <c r="C142" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D142" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:4">
-      <c r="A143" s="45">
+      <c r="A143" s="41">
         <v>3744</v>
       </c>
-      <c r="B143" s="45">
+      <c r="B143" s="41">
         <v>266916</v>
       </c>
-      <c r="C143" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D143" s="45" t="s">
+      <c r="C143" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D143" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:4">
-      <c r="A144" s="45">
+      <c r="A144" s="41">
         <v>3840</v>
       </c>
-      <c r="B144" s="45">
+      <c r="B144" s="41">
         <v>273760</v>
       </c>
-      <c r="C144" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D144" s="45" t="s">
+      <c r="C144" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D144" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:4">
-      <c r="A145" s="45">
+      <c r="A145" s="41">
         <v>3936</v>
       </c>
-      <c r="B145" s="45">
+      <c r="B145" s="41">
         <v>280604</v>
       </c>
-      <c r="C145" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D145" s="45" t="s">
+      <c r="C145" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D145" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:4">
-      <c r="A146" s="45">
+      <c r="A146" s="41">
         <v>4032</v>
       </c>
-      <c r="B146" s="45">
+      <c r="B146" s="41">
         <v>287448</v>
       </c>
-      <c r="C146" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D146" s="45" t="s">
+      <c r="C146" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D146" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:4">
-      <c r="A147" s="45">
+      <c r="A147" s="41">
         <v>4128</v>
       </c>
-      <c r="B147" s="45">
+      <c r="B147" s="41">
         <v>294292</v>
       </c>
-      <c r="C147" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D147" s="45" t="s">
+      <c r="C147" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D147" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:4">
-      <c r="A148" s="45">
+      <c r="A148" s="41">
         <v>4224</v>
       </c>
-      <c r="B148" s="45">
+      <c r="B148" s="41">
         <v>301136</v>
       </c>
-      <c r="C148" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D148" s="45" t="s">
+      <c r="C148" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D148" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:4">
-      <c r="A149" s="45">
+      <c r="A149" s="41">
         <v>4320</v>
       </c>
-      <c r="B149" s="45">
+      <c r="B149" s="41">
         <v>307980</v>
       </c>
-      <c r="C149" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D149" s="45" t="s">
+      <c r="C149" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D149" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:4">
-      <c r="A150" s="45">
+      <c r="A150" s="41">
         <v>4416</v>
       </c>
-      <c r="B150" s="45">
+      <c r="B150" s="41">
         <v>314824</v>
       </c>
-      <c r="C150" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D150" s="45" t="s">
+      <c r="C150" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D150" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:4">
-      <c r="A151" s="45">
+      <c r="A151" s="41">
         <v>4512</v>
       </c>
-      <c r="B151" s="45">
+      <c r="B151" s="41">
         <v>321668</v>
       </c>
-      <c r="C151" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D151" s="45" t="s">
+      <c r="C151" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D151" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:4">
-      <c r="A152" s="45">
+      <c r="A152" s="41">
         <v>4608</v>
       </c>
-      <c r="B152" s="45">
+      <c r="B152" s="41">
         <v>328512</v>
       </c>
-      <c r="C152" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D152" s="45" t="s">
+      <c r="C152" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D152" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:4">
-      <c r="A153" s="45">
+      <c r="A153" s="41">
         <v>4704</v>
       </c>
-      <c r="B153" s="45">
+      <c r="B153" s="41">
         <v>335356</v>
       </c>
-      <c r="C153" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D153" s="45" t="s">
+      <c r="C153" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D153" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:4">
-      <c r="A154" s="45">
+      <c r="A154" s="41">
         <v>4800</v>
       </c>
-      <c r="B154" s="45">
+      <c r="B154" s="41">
         <v>342200</v>
       </c>
-      <c r="C154" s="45">
-        <v>71.291666669999998</v>
-      </c>
-      <c r="D154" s="45" t="s">
+      <c r="C154" s="41">
+        <v>71.291666669999998</v>
+      </c>
+      <c r="D154" s="41" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>